<commit_message>
added Coil CAD; updated list of material; updated guide; fixed 1p ctrl PR
</commit_message>
<xml_diff>
--- a/3. Design/existências.xlsx
+++ b/3. Design/existências.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
   <si>
     <t>Description</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>???</t>
-  </si>
-  <si>
-    <t>ERP</t>
   </si>
   <si>
     <t>NOT</t>
@@ -641,17 +638,48 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -681,6 +709,37 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -803,68 +862,6 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
@@ -984,13 +981,13 @@
     <tableColumn id="1" name="fornecedor" dataDxfId="9"/>
     <tableColumn id="2" name="VPN" dataDxfId="8"/>
     <tableColumn id="3" name="Description" dataDxfId="7"/>
-    <tableColumn id="4" name="Qnt_inv" dataDxfId="4"/>
-    <tableColumn id="5" name="Qnt_ctrl" dataDxfId="3"/>
-    <tableColumn id="6" name="qnt_total" dataDxfId="2"/>
-    <tableColumn id="8" name="existências FEUP" dataDxfId="0"/>
-    <tableColumn id="9" name="comentários" dataDxfId="1"/>
-    <tableColumn id="10" name="capacidade de construçãod e novos conversores" dataDxfId="6"/>
-    <tableColumn id="11" name="componente crítico?" dataDxfId="5"/>
+    <tableColumn id="4" name="Qnt_inv" dataDxfId="6"/>
+    <tableColumn id="5" name="Qnt_ctrl" dataDxfId="5"/>
+    <tableColumn id="6" name="qnt_total" dataDxfId="4"/>
+    <tableColumn id="8" name="existências FEUP" dataDxfId="3"/>
+    <tableColumn id="9" name="comentários" dataDxfId="2"/>
+    <tableColumn id="10" name="capacidade de construçãod e novos conversores" dataDxfId="1"/>
+    <tableColumn id="11" name="componente crítico?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,8 +1258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1303,13 +1300,13 @@
         <v>87</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1340,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1362,11 +1359,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="23" t="s">
         <v>86</v>
@@ -1394,10 +1391,10 @@
         <v>4</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>86</v>
@@ -1422,11 +1419,11 @@
         <v>10</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>86</v>
@@ -1453,11 +1450,11 @@
         <v>12</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>86</v>
@@ -1484,11 +1481,11 @@
         <v>8</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>86</v>
@@ -1578,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1600,11 +1597,11 @@
         <v>3</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J11" s="23" t="s">
         <v>86</v>
@@ -1628,12 +1625,12 @@
         <v>16</v>
       </c>
       <c r="G12" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="29"/>
       <c r="J12" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1654,13 +1651,13 @@
         <f t="shared" ref="F13" si="1">E13+D13</f>
         <v>8</v>
       </c>
-      <c r="G13" s="27" t="s">
-        <v>93</v>
+      <c r="G13" s="27">
+        <v>10</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="29"/>
       <c r="J13" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,7 +1710,7 @@
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>86</v>
@@ -1767,13 +1764,13 @@
         <v>9</v>
       </c>
       <c r="G17" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>103</v>
-      </c>
       <c r="I17" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>86</v>
@@ -1802,7 +1799,7 @@
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>86</v>
@@ -1830,10 +1827,10 @@
         <v>10</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J19" s="23" t="s">
         <v>86</v>
@@ -1863,10 +1860,10 @@
         <v>10</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J20" s="23" t="s">
         <v>86</v>
@@ -1894,10 +1891,10 @@
         <v>10</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J21" s="23" t="s">
         <v>86</v>
@@ -1927,10 +1924,10 @@
         <v>10</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J22" s="23" t="s">
         <v>86</v>
@@ -1958,10 +1955,10 @@
         <v>17</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J23" s="23" t="s">
         <v>86</v>
@@ -2022,10 +2019,10 @@
         <v>35</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J25" s="23" t="s">
         <v>86</v>
@@ -2055,10 +2052,10 @@
         <v>30</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J26" s="23" t="s">
         <v>86</v>
@@ -2149,7 +2146,7 @@
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J29" s="23" t="s">
         <v>86</v>
@@ -2174,11 +2171,11 @@
         <v>4</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J30" s="23" t="s">
         <v>86</v>
@@ -2207,7 +2204,7 @@
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J31" s="23" t="s">
         <v>86</v>
@@ -2235,10 +2232,10 @@
         <v>54</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J32" s="23" t="s">
         <v>86</v>
@@ -2301,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2385,7 +2382,7 @@
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>86</v>
@@ -2414,10 +2411,10 @@
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2504,7 +2501,7 @@
         <v>91</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Completed alfa version of REV 3.0
developed 3 boards plus the CAD asm
</commit_message>
<xml_diff>
--- a/3. Design/existências.xlsx
+++ b/3. Design/existências.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="115">
   <si>
     <t>Description</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>???</t>
-  </si>
-  <si>
-    <t>NOT</t>
   </si>
   <si>
     <t>60++</t>
@@ -1258,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1300,13 +1297,13 @@
         <v>87</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1337,7 +1334,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1359,11 +1356,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J3" s="23" t="s">
         <v>86</v>
@@ -1391,10 +1388,10 @@
         <v>4</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J4" s="23" t="s">
         <v>86</v>
@@ -1419,11 +1416,11 @@
         <v>10</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J5" s="23" t="s">
         <v>86</v>
@@ -1450,11 +1447,11 @@
         <v>12</v>
       </c>
       <c r="G6" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J6" s="23" t="s">
         <v>86</v>
@@ -1481,11 +1478,11 @@
         <v>8</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" s="23" t="s">
         <v>86</v>
@@ -1575,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,11 +1594,11 @@
         <v>3</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J11" s="23" t="s">
         <v>86</v>
@@ -1624,13 +1621,13 @@
       <c r="F12" s="21">
         <v>16</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>93</v>
+      <c r="G12" s="26">
+        <v>19</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="29"/>
       <c r="J12" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1657,7 +1654,7 @@
       <c r="H13" s="23"/>
       <c r="I13" s="29"/>
       <c r="J13" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1710,7 +1707,7 @@
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>86</v>
@@ -1764,13 +1761,13 @@
         <v>9</v>
       </c>
       <c r="G17" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>102</v>
-      </c>
       <c r="I17" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>86</v>
@@ -1799,7 +1796,7 @@
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>86</v>
@@ -1827,10 +1824,10 @@
         <v>10</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J19" s="23" t="s">
         <v>86</v>
@@ -1860,10 +1857,10 @@
         <v>10</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J20" s="23" t="s">
         <v>86</v>
@@ -1891,10 +1888,10 @@
         <v>10</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J21" s="23" t="s">
         <v>86</v>
@@ -1924,10 +1921,10 @@
         <v>10</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J22" s="23" t="s">
         <v>86</v>
@@ -1955,10 +1952,10 @@
         <v>17</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I23" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J23" s="23" t="s">
         <v>86</v>
@@ -2019,10 +2016,10 @@
         <v>35</v>
       </c>
       <c r="H25" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J25" s="23" t="s">
         <v>86</v>
@@ -2052,10 +2049,10 @@
         <v>30</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J26" s="23" t="s">
         <v>86</v>
@@ -2146,7 +2143,7 @@
       </c>
       <c r="H29" s="23"/>
       <c r="I29" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J29" s="23" t="s">
         <v>86</v>
@@ -2171,11 +2168,11 @@
         <v>4</v>
       </c>
       <c r="G30" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H30" s="23"/>
       <c r="I30" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J30" s="23" t="s">
         <v>86</v>
@@ -2204,7 +2201,7 @@
       </c>
       <c r="H31" s="23"/>
       <c r="I31" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J31" s="23" t="s">
         <v>86</v>
@@ -2232,10 +2229,10 @@
         <v>54</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I32" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J32" s="23" t="s">
         <v>86</v>
@@ -2298,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2382,7 +2379,7 @@
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>86</v>
@@ -2411,10 +2408,10 @@
       </c>
       <c r="H38" s="23"/>
       <c r="I38" s="29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2501,7 +2498,7 @@
         <v>91</v>
       </c>
       <c r="I41" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
ammendment on PCBs and preliminary CAD generation
</commit_message>
<xml_diff>
--- a/3. Design/existências.xlsx
+++ b/3. Design/existências.xlsx
@@ -1255,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2077,11 +2077,11 @@
         <v>1</v>
       </c>
       <c r="G27" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" s="23"/>
-      <c r="I27" s="29">
-        <v>2</v>
+      <c r="I27" s="31">
+        <v>1</v>
       </c>
       <c r="J27" s="23" t="s">
         <v>86</v>

</xml_diff>